<commit_message>
Updated figures and added new slides
</commit_message>
<xml_diff>
--- a/outputs/crossValV2/f1Report.xlsx
+++ b/outputs/crossValV2/f1Report.xlsx
@@ -8,13 +8,95 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lando\Documents\GitHub\Buell-Masters-Project\outputs\crossValV2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BC3A58F-0923-4113-A070-4A932F6FD151}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10E1C15E-FFAB-4195-8239-EB48CEFE2DBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25180" windowHeight="16260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25200" windowHeight="16280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$C$2</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$C$3:$C$31</definedName>
+    <definedName name="_xlchart.v1.10" hidden="1">Sheet1!$H$2</definedName>
+    <definedName name="_xlchart.v1.11" hidden="1">Sheet1!$H$3:$H$31</definedName>
+    <definedName name="_xlchart.v1.12" hidden="1">Sheet1!$I$2</definedName>
+    <definedName name="_xlchart.v1.13" hidden="1">Sheet1!$I$3:$I$31</definedName>
+    <definedName name="_xlchart.v1.14" hidden="1">Sheet1!$J$2</definedName>
+    <definedName name="_xlchart.v1.15" hidden="1">Sheet1!$J$3:$J$31</definedName>
+    <definedName name="_xlchart.v1.16" hidden="1">Sheet1!$K$2</definedName>
+    <definedName name="_xlchart.v1.17" hidden="1">Sheet1!$K$3:$K$31</definedName>
+    <definedName name="_xlchart.v1.18" hidden="1">Sheet1!$L$2</definedName>
+    <definedName name="_xlchart.v1.19" hidden="1">Sheet1!$L$3:$L$31</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$D$2</definedName>
+    <definedName name="_xlchart.v1.20" hidden="1">Sheet1!$C$2</definedName>
+    <definedName name="_xlchart.v1.21" hidden="1">Sheet1!$C$3:$C$31</definedName>
+    <definedName name="_xlchart.v1.22" hidden="1">Sheet1!$D$2</definedName>
+    <definedName name="_xlchart.v1.23" hidden="1">Sheet1!$D$3:$D$31</definedName>
+    <definedName name="_xlchart.v1.24" hidden="1">Sheet1!$E$2</definedName>
+    <definedName name="_xlchart.v1.25" hidden="1">Sheet1!$E$3:$E$31</definedName>
+    <definedName name="_xlchart.v1.26" hidden="1">Sheet1!$F$2</definedName>
+    <definedName name="_xlchart.v1.27" hidden="1">Sheet1!$F$3:$F$31</definedName>
+    <definedName name="_xlchart.v1.28" hidden="1">Sheet1!$G$2</definedName>
+    <definedName name="_xlchart.v1.29" hidden="1">Sheet1!$G$3:$G$31</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">Sheet1!$D$3:$D$31</definedName>
+    <definedName name="_xlchart.v1.30" hidden="1">Sheet1!$H$2</definedName>
+    <definedName name="_xlchart.v1.31" hidden="1">Sheet1!$H$3:$H$31</definedName>
+    <definedName name="_xlchart.v1.32" hidden="1">Sheet1!$I$2</definedName>
+    <definedName name="_xlchart.v1.33" hidden="1">Sheet1!$I$3:$I$31</definedName>
+    <definedName name="_xlchart.v1.34" hidden="1">Sheet1!$J$2</definedName>
+    <definedName name="_xlchart.v1.35" hidden="1">Sheet1!$J$3:$J$31</definedName>
+    <definedName name="_xlchart.v1.36" hidden="1">Sheet1!$K$2</definedName>
+    <definedName name="_xlchart.v1.37" hidden="1">Sheet1!$K$3:$K$31</definedName>
+    <definedName name="_xlchart.v1.38" hidden="1">Sheet1!$L$2</definedName>
+    <definedName name="_xlchart.v1.39" hidden="1">Sheet1!$L$3:$L$31</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">Sheet1!$E$2</definedName>
+    <definedName name="_xlchart.v1.40" hidden="1">Sheet1!$C$2</definedName>
+    <definedName name="_xlchart.v1.41" hidden="1">Sheet1!$C$3:$C$31</definedName>
+    <definedName name="_xlchart.v1.42" hidden="1">Sheet1!$D$2</definedName>
+    <definedName name="_xlchart.v1.43" hidden="1">Sheet1!$D$3:$D$31</definedName>
+    <definedName name="_xlchart.v1.44" hidden="1">Sheet1!$E$2</definedName>
+    <definedName name="_xlchart.v1.45" hidden="1">Sheet1!$E$3:$E$31</definedName>
+    <definedName name="_xlchart.v1.46" hidden="1">Sheet1!$F$2</definedName>
+    <definedName name="_xlchart.v1.47" hidden="1">Sheet1!$F$3:$F$31</definedName>
+    <definedName name="_xlchart.v1.48" hidden="1">Sheet1!$G$2</definedName>
+    <definedName name="_xlchart.v1.49" hidden="1">Sheet1!$G$3:$G$31</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">Sheet1!$E$3:$E$31</definedName>
+    <definedName name="_xlchart.v1.50" hidden="1">Sheet1!$H$2</definedName>
+    <definedName name="_xlchart.v1.51" hidden="1">Sheet1!$H$3:$H$31</definedName>
+    <definedName name="_xlchart.v1.52" hidden="1">Sheet1!$I$2</definedName>
+    <definedName name="_xlchart.v1.53" hidden="1">Sheet1!$I$3:$I$31</definedName>
+    <definedName name="_xlchart.v1.54" hidden="1">Sheet1!$J$2</definedName>
+    <definedName name="_xlchart.v1.55" hidden="1">Sheet1!$J$3:$J$31</definedName>
+    <definedName name="_xlchart.v1.56" hidden="1">Sheet1!$K$2</definedName>
+    <definedName name="_xlchart.v1.57" hidden="1">Sheet1!$K$3:$K$31</definedName>
+    <definedName name="_xlchart.v1.58" hidden="1">Sheet1!$L$2</definedName>
+    <definedName name="_xlchart.v1.59" hidden="1">Sheet1!$L$3:$L$31</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">Sheet1!$F$2</definedName>
+    <definedName name="_xlchart.v1.60" hidden="1">Sheet1!$C$2</definedName>
+    <definedName name="_xlchart.v1.61" hidden="1">Sheet1!$C$3:$C$31</definedName>
+    <definedName name="_xlchart.v1.62" hidden="1">Sheet1!$D$2</definedName>
+    <definedName name="_xlchart.v1.63" hidden="1">Sheet1!$D$3:$D$31</definedName>
+    <definedName name="_xlchart.v1.64" hidden="1">Sheet1!$E$2</definedName>
+    <definedName name="_xlchart.v1.65" hidden="1">Sheet1!$E$3:$E$31</definedName>
+    <definedName name="_xlchart.v1.66" hidden="1">Sheet1!$F$2</definedName>
+    <definedName name="_xlchart.v1.67" hidden="1">Sheet1!$F$3:$F$31</definedName>
+    <definedName name="_xlchart.v1.68" hidden="1">Sheet1!$G$2</definedName>
+    <definedName name="_xlchart.v1.69" hidden="1">Sheet1!$G$3:$G$31</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">Sheet1!$F$3:$F$31</definedName>
+    <definedName name="_xlchart.v1.70" hidden="1">Sheet1!$H$2</definedName>
+    <definedName name="_xlchart.v1.71" hidden="1">Sheet1!$H$3:$H$31</definedName>
+    <definedName name="_xlchart.v1.72" hidden="1">Sheet1!$I$2</definedName>
+    <definedName name="_xlchart.v1.73" hidden="1">Sheet1!$I$3:$I$31</definedName>
+    <definedName name="_xlchart.v1.74" hidden="1">Sheet1!$J$2</definedName>
+    <definedName name="_xlchart.v1.75" hidden="1">Sheet1!$J$3:$J$31</definedName>
+    <definedName name="_xlchart.v1.76" hidden="1">Sheet1!$K$2</definedName>
+    <definedName name="_xlchart.v1.77" hidden="1">Sheet1!$K$3:$K$31</definedName>
+    <definedName name="_xlchart.v1.78" hidden="1">Sheet1!$L$2</definedName>
+    <definedName name="_xlchart.v1.79" hidden="1">Sheet1!$L$3:$L$31</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">Sheet1!$G$2</definedName>
+    <definedName name="_xlchart.v1.9" hidden="1">Sheet1!$G$3:$G$31</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -276,6 +358,875 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chartEx1.xml><?xml version="1.0" encoding="utf-8"?>
+<cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
+  <cx:chartData>
+    <cx:data id="0">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.41</cx:f>
+      </cx:numDim>
+    </cx:data>
+    <cx:data id="1">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.43</cx:f>
+      </cx:numDim>
+    </cx:data>
+    <cx:data id="2">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.45</cx:f>
+      </cx:numDim>
+    </cx:data>
+    <cx:data id="3">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.47</cx:f>
+      </cx:numDim>
+    </cx:data>
+    <cx:data id="4">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.49</cx:f>
+      </cx:numDim>
+    </cx:data>
+    <cx:data id="5">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.51</cx:f>
+      </cx:numDim>
+    </cx:data>
+    <cx:data id="6">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.53</cx:f>
+      </cx:numDim>
+    </cx:data>
+    <cx:data id="7">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.55</cx:f>
+      </cx:numDim>
+    </cx:data>
+    <cx:data id="8">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.57</cx:f>
+      </cx:numDim>
+    </cx:data>
+    <cx:data id="9">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.59</cx:f>
+      </cx:numDim>
+    </cx:data>
+  </cx:chartData>
+  <cx:chart>
+    <cx:title pos="t" align="ctr" overlay="0">
+      <cx:tx>
+        <cx:txData>
+          <cx:v>F1-Score By Cross Validation Fold</cx:v>
+        </cx:txData>
+      </cx:tx>
+      <cx:txPr>
+        <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:sysClr>
+              </a:solidFill>
+              <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+            </a:rPr>
+            <a:t>F1-Score By Cross Validation Fold</a:t>
+          </a:r>
+        </a:p>
+      </cx:txPr>
+    </cx:title>
+    <cx:plotArea>
+      <cx:plotAreaRegion>
+        <cx:series layoutId="boxWhisker" uniqueId="{B06E929B-EA50-4EBF-B00F-B29B4BCD2A67}">
+          <cx:tx>
+            <cx:txData>
+              <cx:f>_xlchart.v1.40</cx:f>
+              <cx:v>fold 0</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:dataId val="0"/>
+          <cx:layoutPr>
+            <cx:visibility meanLine="1" meanMarker="1" nonoutliers="0" outliers="1"/>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+        <cx:series layoutId="boxWhisker" uniqueId="{0DD99CE4-3A6B-438F-A61B-6253B560AFF5}">
+          <cx:tx>
+            <cx:txData>
+              <cx:f>_xlchart.v1.42</cx:f>
+              <cx:v>fold 1</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:dataId val="1"/>
+          <cx:layoutPr>
+            <cx:visibility meanLine="1" meanMarker="1" nonoutliers="0" outliers="1"/>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+        <cx:series layoutId="boxWhisker" uniqueId="{8A0ACBDF-C44C-48D3-A41E-4C39B6CF7BDA}">
+          <cx:tx>
+            <cx:txData>
+              <cx:f>_xlchart.v1.44</cx:f>
+              <cx:v>fold 2</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:dataId val="2"/>
+          <cx:layoutPr>
+            <cx:visibility meanLine="1" meanMarker="1" nonoutliers="0" outliers="1"/>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+        <cx:series layoutId="boxWhisker" uniqueId="{5A601667-EEF5-4785-A906-080A90E775B7}">
+          <cx:tx>
+            <cx:txData>
+              <cx:f>_xlchart.v1.46</cx:f>
+              <cx:v>fold 3</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:dataId val="3"/>
+          <cx:layoutPr>
+            <cx:visibility meanLine="1" meanMarker="1" nonoutliers="0" outliers="1"/>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+        <cx:series layoutId="boxWhisker" uniqueId="{51A69567-7053-4D92-A60E-981F2470B1DC}">
+          <cx:tx>
+            <cx:txData>
+              <cx:f>_xlchart.v1.48</cx:f>
+              <cx:v>fold 4</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:dataId val="4"/>
+          <cx:layoutPr>
+            <cx:visibility meanLine="1" meanMarker="1" nonoutliers="0" outliers="1"/>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+        <cx:series layoutId="boxWhisker" uniqueId="{7BF8BC2F-56D4-4F76-BFF7-33BE469BBB93}">
+          <cx:tx>
+            <cx:txData>
+              <cx:f>_xlchart.v1.50</cx:f>
+              <cx:v>fold 5</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:dataId val="5"/>
+          <cx:layoutPr>
+            <cx:visibility meanLine="1" meanMarker="1" nonoutliers="0" outliers="1"/>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+        <cx:series layoutId="boxWhisker" uniqueId="{ED19DD5D-C9DE-4C9C-B179-9A15F26BE0BD}">
+          <cx:tx>
+            <cx:txData>
+              <cx:f>_xlchart.v1.52</cx:f>
+              <cx:v>fold 6</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:dataId val="6"/>
+          <cx:layoutPr>
+            <cx:visibility meanLine="1" meanMarker="1" nonoutliers="0" outliers="1"/>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+        <cx:series layoutId="boxWhisker" uniqueId="{37303681-990F-4909-B3A9-470C34505440}">
+          <cx:tx>
+            <cx:txData>
+              <cx:f>_xlchart.v1.54</cx:f>
+              <cx:v>fold 7</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:dataId val="7"/>
+          <cx:layoutPr>
+            <cx:visibility meanLine="1" meanMarker="1" nonoutliers="0" outliers="1"/>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+        <cx:series layoutId="boxWhisker" uniqueId="{19C71632-D5F3-42F8-A633-7FE9F7966F51}">
+          <cx:tx>
+            <cx:txData>
+              <cx:f>_xlchart.v1.56</cx:f>
+              <cx:v>fold 8</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:dataId val="8"/>
+          <cx:layoutPr>
+            <cx:visibility meanLine="1" meanMarker="1" nonoutliers="0" outliers="1"/>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+        <cx:series layoutId="boxWhisker" uniqueId="{F047C7B3-179F-4FF3-9F67-DBB28DC69872}">
+          <cx:tx>
+            <cx:txData>
+              <cx:f>_xlchart.v1.58</cx:f>
+              <cx:v>fold 9</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:dataId val="9"/>
+          <cx:layoutPr>
+            <cx:visibility meanLine="1" meanMarker="1" nonoutliers="0" outliers="1"/>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+      </cx:plotAreaRegion>
+      <cx:axis id="0" hidden="1">
+        <cx:catScaling gapWidth="0.100000001"/>
+        <cx:tickLabels/>
+      </cx:axis>
+      <cx:axis id="1">
+        <cx:valScaling/>
+        <cx:majorGridlines/>
+        <cx:tickLabels/>
+      </cx:axis>
+    </cx:plotArea>
+    <cx:legend pos="b" align="ctr" overlay="0"/>
+  </cx:chart>
+</cx:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="373">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat">
+        <a:solidFill>
+          <a:srgbClr val="D9D9D9"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>31750</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>31750</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="2" name="Chart 1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B6F0316C-78AE-4C2D-AB71-A1937B032659}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
+              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="9359900" y="254000"/>
+              <a:ext cx="7315200" cy="3657600"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100"/>
+                <a:t>This chart isn't available in your version of Excel.
+Editing this shape or saving this workbook into a different file format will permanently break the chart.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -543,8 +1494,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P6" sqref="P6"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="Q24" sqref="Q24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2049,5 +3000,6 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>